<commit_message>
20250319 AEXEW BNEW CLEW CACEW in compare
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202503/Blue chip review checklist March 2025.xlsx
+++ b/GUI + Reviews/202503/Blue chip review checklist March 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202503\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB279C51-5423-4217-AEB7-6818886D436E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809922B2-80BF-4B7A-84D7-D8B272421C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="84">
   <si>
     <t>Review check list blue chip family review</t>
   </si>
@@ -261,9 +261,6 @@
     <t>CAC</t>
   </si>
   <si>
-    <t>09-12-2024 until 12-12-2024</t>
-  </si>
-  <si>
     <t>27-01-25 until 21-02-25</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>11-03-25 until 13-03-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB </t>
   </si>
 </sst>
 </file>
@@ -829,10 +829,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96:G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -993,7 +993,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
@@ -1315,7 +1315,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>68</v>
@@ -1376,7 +1376,7 @@
         <v>75</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>64</v>
@@ -1460,7 +1460,7 @@
       <c r="A32" s="14"/>
       <c r="B32" s="31"/>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="2" t="s">
@@ -1482,7 +1482,7 @@
         <v>75</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>17</v>
@@ -1566,7 +1566,7 @@
       <c r="A38" s="14"/>
       <c r="B38" s="31"/>
       <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="2" t="s">
@@ -1588,7 +1588,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>68</v>
@@ -1609,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>6</v>
@@ -1630,7 +1630,7 @@
         <v>75</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>68</v>
@@ -1731,7 +1731,7 @@
       <c r="A47" s="14"/>
       <c r="B47" s="31"/>
       <c r="C47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D47" s="28"/>
       <c r="E47" s="2" t="s">
@@ -1753,10 +1753,10 @@
         <v>6</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>57</v>
@@ -1774,10 +1774,10 @@
         <v>6</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>57</v>
@@ -1795,7 +1795,7 @@
         <v>75</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>64</v>
@@ -1879,11 +1879,11 @@
       <c r="A55" s="14"/>
       <c r="B55" s="31"/>
       <c r="C55" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55" s="28"/>
       <c r="E55" s="2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>57</v>
@@ -1901,7 +1901,7 @@
         <v>75</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -1985,11 +1985,11 @@
       <c r="A61" s="14"/>
       <c r="B61" s="20"/>
       <c r="C61" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>57</v>
@@ -2007,7 +2007,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>6</v>
@@ -2028,7 +2028,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="3">
-        <v>45644</v>
+        <v>45735</v>
       </c>
       <c r="E63" s="18"/>
       <c r="F63" s="18" t="s">
@@ -2047,17 +2047,13 @@
         <v>75</v>
       </c>
       <c r="D64" s="27">
-        <v>45644</v>
+        <v>45735</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
@@ -2069,12 +2065,8 @@
       <c r="E65" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F65" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
@@ -2086,12 +2078,8 @@
       <c r="E66" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F66" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
@@ -2103,12 +2091,8 @@
       <c r="E67" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F67" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="14"/>
@@ -2118,520 +2102,404 @@
       </c>
       <c r="D68" s="28"/>
       <c r="E68" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
-      <c r="B69" s="24" t="s">
-        <v>36</v>
-      </c>
+      <c r="A69" s="14"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D69" s="27">
-        <v>45644</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D69" s="28"/>
       <c r="E69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F69" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="31"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="C70" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D70" s="27">
+        <v>45735</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F70" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="14"/>
       <c r="B71" s="31"/>
       <c r="C71" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D71" s="28"/>
       <c r="E71" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="14"/>
       <c r="B72" s="31"/>
       <c r="C72" s="2" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="D72" s="28"/>
       <c r="E72" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="14"/>
       <c r="B73" s="31"/>
       <c r="C73" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D73" s="28"/>
       <c r="E73" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
     </row>
     <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="11"/>
-      <c r="B74" s="24" t="s">
-        <v>70</v>
-      </c>
+      <c r="A74" s="14"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D74" s="27">
-        <v>45644</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D74" s="28"/>
       <c r="E74" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="11"/>
-      <c r="B75" s="25"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D75" s="28"/>
       <c r="E75" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
     </row>
     <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A76" s="11"/>
-      <c r="B76" s="25"/>
+      <c r="B76" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="C76" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D76" s="27">
+        <v>45735</v>
+      </c>
       <c r="E76" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
       <c r="B77" s="25"/>
       <c r="C77" s="2" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D77" s="28"/>
       <c r="E77" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A78" s="11"/>
       <c r="B78" s="25"/>
       <c r="C78" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D78" s="28"/>
       <c r="E78" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
     </row>
     <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="11"/>
-      <c r="B79" s="24" t="s">
-        <v>37</v>
-      </c>
+      <c r="B79" s="25"/>
       <c r="C79" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="27">
-        <v>45644</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D79" s="28"/>
       <c r="E79" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
     </row>
     <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="11"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="25"/>
       <c r="C80" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D80" s="28"/>
       <c r="E80" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
     </row>
     <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A81" s="11"/>
       <c r="B81" s="25"/>
       <c r="C81" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D81" s="28"/>
       <c r="E81" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
     </row>
     <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A82" s="11"/>
-      <c r="B82" s="25"/>
+      <c r="B82" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="C82" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D82" s="27">
+        <v>45735</v>
+      </c>
       <c r="E82" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
     </row>
     <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
       <c r="B83" s="25"/>
       <c r="C83" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D83" s="28"/>
       <c r="E83" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A84" s="11"/>
-      <c r="B84" s="24" t="s">
-        <v>38</v>
-      </c>
+      <c r="B84" s="25"/>
       <c r="C84" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D84" s="27">
-        <v>45644</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D84" s="28"/>
       <c r="E84" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
     </row>
     <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A85" s="11"/>
       <c r="B85" s="25"/>
       <c r="C85" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D85" s="28"/>
       <c r="E85" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="11"/>
+      <c r="A86" s="14"/>
       <c r="B86" s="25"/>
       <c r="C86" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D86" s="28"/>
       <c r="E86" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F86" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G86" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A87" s="11"/>
       <c r="B87" s="25"/>
       <c r="C87" s="2" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D87" s="28"/>
       <c r="E87" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
     </row>
     <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A88" s="11"/>
-      <c r="B88" s="25"/>
+      <c r="B88" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="C88" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D88" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D88" s="27">
+        <v>45735</v>
+      </c>
       <c r="E88" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A89" s="17"/>
-      <c r="B89" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A89" s="11"/>
+      <c r="B89" s="25"/>
       <c r="C89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="3">
-        <v>45646</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D89" s="28"/>
       <c r="E89" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F89" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="11"/>
+      <c r="B90" s="25"/>
       <c r="C90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="3">
-        <v>45649</v>
-      </c>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G90" s="18" t="s">
-        <v>57</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D90" s="28"/>
+      <c r="E90" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
     </row>
     <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A91" s="11"/>
-      <c r="B91" s="24" t="s">
-        <v>41</v>
-      </c>
+      <c r="B91" s="25"/>
       <c r="C91" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D91" s="27">
-        <v>45646</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D91" s="28"/>
       <c r="E91" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
     </row>
     <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A92" s="11"/>
       <c r="B92" s="25"/>
       <c r="C92" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D92" s="28"/>
       <c r="E92" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F92" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
     </row>
     <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A93" s="11"/>
       <c r="B93" s="25"/>
       <c r="C93" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D93" s="28"/>
       <c r="E93" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
     </row>
     <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="11"/>
-      <c r="B94" s="25"/>
+      <c r="A94" s="17"/>
+      <c r="B94" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C94" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D94" s="28"/>
+        <v>6</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45735</v>
+      </c>
       <c r="E94" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A95" s="11"/>
-      <c r="B95" s="25"/>
+        <v>68</v>
+      </c>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="17"/>
+      <c r="B95" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D95" s="28"/>
-      <c r="E95" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G95" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="3">
+        <v>45737</v>
+      </c>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G95" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A96" s="11"/>
       <c r="B96" s="24" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D96" s="27">
-        <v>45646</v>
+        <v>45737</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
     </row>
     <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A97" s="11"/>
@@ -2641,14 +2509,10 @@
       </c>
       <c r="D97" s="28"/>
       <c r="E97" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
     </row>
     <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A98" s="11"/>
@@ -2658,14 +2522,10 @@
       </c>
       <c r="D98" s="28"/>
       <c r="E98" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G98" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
     </row>
     <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A99" s="11"/>
@@ -2675,14 +2535,10 @@
       </c>
       <c r="D99" s="28"/>
       <c r="E99" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
     </row>
     <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A100" s="11"/>
@@ -2694,445 +2550,493 @@
       <c r="E100" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F100" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G100" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
     </row>
     <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A101" s="11"/>
-      <c r="B101" s="24" t="s">
-        <v>42</v>
-      </c>
+      <c r="B101" s="25"/>
       <c r="C101" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D101" s="27">
-        <v>45646</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D101" s="28"/>
       <c r="E101" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
     </row>
     <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A102" s="11"/>
-      <c r="B102" s="25"/>
+      <c r="B102" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="C102" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D102" s="27">
+        <v>45737</v>
+      </c>
       <c r="E102" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
     </row>
     <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A103" s="11"/>
       <c r="B103" s="25"/>
       <c r="C103" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D103" s="28"/>
       <c r="E103" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
     </row>
     <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A104" s="11"/>
       <c r="B104" s="25"/>
       <c r="C104" s="2" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="D104" s="28"/>
       <c r="E104" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
     </row>
     <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A105" s="11"/>
       <c r="B105" s="25"/>
       <c r="C105" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D105" s="28"/>
       <c r="E105" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
     </row>
     <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A106" s="11"/>
-      <c r="B106" s="24" t="s">
-        <v>50</v>
-      </c>
+      <c r="B106" s="25"/>
       <c r="C106" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D106" s="27">
-        <v>45646</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D106" s="28"/>
       <c r="E106" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F106" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G106" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A107" s="11"/>
       <c r="B107" s="25"/>
       <c r="C107" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D107" s="28"/>
       <c r="E107" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G107" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
     </row>
     <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A108" s="11"/>
-      <c r="B108" s="25"/>
+      <c r="B108" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="C108" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D108" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D108" s="27">
+        <v>45737</v>
+      </c>
       <c r="E108" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
     </row>
     <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A109" s="11"/>
       <c r="B109" s="25"/>
       <c r="C109" s="2" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D109" s="28"/>
       <c r="E109" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F109" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
     </row>
     <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A110" s="11"/>
       <c r="B110" s="25"/>
       <c r="C110" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D110" s="28"/>
       <c r="E110" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F110" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
     </row>
     <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A111" s="17"/>
-      <c r="B111" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A111" s="11"/>
+      <c r="B111" s="25"/>
       <c r="C111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" s="3">
-        <v>45646</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D111" s="28"/>
       <c r="E111" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
     </row>
     <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A112" s="11"/>
-      <c r="B112" s="24" t="s">
-        <v>44</v>
-      </c>
+      <c r="B112" s="25"/>
       <c r="C112" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D112" s="27">
-        <v>45646</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D112" s="28"/>
       <c r="E112" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
     </row>
     <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A113" s="11"/>
       <c r="B113" s="25"/>
       <c r="C113" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D113" s="28"/>
       <c r="E113" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G113" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
     </row>
     <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A114" s="11"/>
-      <c r="B114" s="25"/>
+      <c r="B114" s="24" t="s">
+        <v>50</v>
+      </c>
       <c r="C114" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D114" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="D114" s="27">
+        <v>45737</v>
+      </c>
       <c r="E114" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
     </row>
     <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A115" s="11"/>
       <c r="B115" s="25"/>
       <c r="C115" s="2" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D115" s="28"/>
       <c r="E115" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
     </row>
     <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A116" s="11"/>
       <c r="B116" s="25"/>
       <c r="C116" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D116" s="28"/>
       <c r="E116" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
     </row>
     <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A117" s="17"/>
-      <c r="B117" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="A117" s="11"/>
+      <c r="B117" s="25"/>
       <c r="C117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="3">
-        <v>45646</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D117" s="28"/>
       <c r="E117" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
     </row>
     <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A118" s="11"/>
-      <c r="B118" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="B118" s="25"/>
       <c r="C118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="3">
-        <v>45646</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D118" s="28"/>
       <c r="E118" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G118" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="22"/>
+        <v>68</v>
+      </c>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A119" s="11"/>
       <c r="B119" s="25"/>
       <c r="C119" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D119" s="28"/>
       <c r="E119" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A120" s="17"/>
+      <c r="B120" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" s="3">
+        <v>45737</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A121" s="11"/>
+      <c r="B121" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D121" s="27">
+        <v>45737</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A122" s="11"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="28"/>
+      <c r="E122" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A123" s="11"/>
+      <c r="B123" s="25"/>
+      <c r="C123" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123" s="28"/>
+      <c r="E123" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="11"/>
+      <c r="B124" s="25"/>
+      <c r="C124" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D124" s="28"/>
+      <c r="E124" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="11"/>
+      <c r="B125" s="25"/>
+      <c r="C125" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="28"/>
+      <c r="E125" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A126" s="11"/>
+      <c r="B126" s="25"/>
+      <c r="C126" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D126" s="28"/>
+      <c r="E126" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A127" s="17"/>
+      <c r="B127" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" s="3">
+        <v>45737</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A128" s="11"/>
+      <c r="B128" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="3">
+        <v>45737</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+    </row>
+    <row r="129" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="22"/>
+      <c r="B129" s="25"/>
+      <c r="C129" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="27"/>
+      <c r="E129" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F119" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G119" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="22"/>
-      <c r="B120" s="25"/>
-      <c r="C120" s="2" t="s">
+      <c r="F129" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="22"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D120" s="28"/>
-      <c r="E120" s="2" t="s">
+      <c r="D130" s="28"/>
+      <c r="E130" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
-      <c r="B121" s="26"/>
-      <c r="C121" s="2" t="s">
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+    </row>
+    <row r="131" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="23"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D121" s="29"/>
-      <c r="E121" s="2" t="s">
+      <c r="D131" s="29"/>
+      <c r="E131" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="12">
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+    </row>
+    <row r="132" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="12">
         <v>59</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="3">
+      <c r="C132" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D132" s="3">
         <v>43084</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E132" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
-    </row>
-    <row r="123" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12">
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+    </row>
+    <row r="133" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="12">
         <v>60</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" s="3">
+      <c r="C133" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="3">
         <v>43084</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="E133" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="129" x14ac:dyDescent="0.25"/>
-    <row r="130" x14ac:dyDescent="0.25"/>
-    <row r="131" x14ac:dyDescent="0.25"/>
-    <row r="132" x14ac:dyDescent="0.25"/>
-    <row r="133" x14ac:dyDescent="0.25"/>
-    <row r="134" x14ac:dyDescent="0.25"/>
-    <row r="135" x14ac:dyDescent="0.25"/>
-    <row r="136" x14ac:dyDescent="0.25"/>
-    <row r="137" x14ac:dyDescent="0.25"/>
-    <row r="138" x14ac:dyDescent="0.25"/>
-    <row r="139" x14ac:dyDescent="0.25"/>
-    <row r="140" x14ac:dyDescent="0.25"/>
-    <row r="141" x14ac:dyDescent="0.25"/>
-    <row r="142" x14ac:dyDescent="0.25"/>
-    <row r="143" x14ac:dyDescent="0.25"/>
-    <row r="144" x14ac:dyDescent="0.25"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25"/>
     <row r="145" x14ac:dyDescent="0.25"/>
     <row r="146" x14ac:dyDescent="0.25"/>
     <row r="147" x14ac:dyDescent="0.25"/>
@@ -3168,41 +3072,51 @@
     <row r="177" x14ac:dyDescent="0.25"/>
     <row r="178" x14ac:dyDescent="0.25"/>
     <row r="179" x14ac:dyDescent="0.25"/>
+    <row r="180" x14ac:dyDescent="0.25"/>
+    <row r="181" x14ac:dyDescent="0.25"/>
+    <row r="182" x14ac:dyDescent="0.25"/>
+    <row r="183" x14ac:dyDescent="0.25"/>
+    <row r="184" x14ac:dyDescent="0.25"/>
+    <row r="185" x14ac:dyDescent="0.25"/>
+    <row r="186" x14ac:dyDescent="0.25"/>
+    <row r="187" x14ac:dyDescent="0.25"/>
+    <row r="188" x14ac:dyDescent="0.25"/>
+    <row r="189" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="33">
     <mergeCell ref="B50:B55"/>
     <mergeCell ref="D50:D55"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="D70:D75"/>
     <mergeCell ref="B56:B59"/>
     <mergeCell ref="D56:D59"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="B64:B69"/>
+    <mergeCell ref="D64:D69"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="D27:D32"/>
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="D33:D38"/>
     <mergeCell ref="B41:B47"/>
     <mergeCell ref="D41:D47"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="D91:D95"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="D96:D100"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B106:B110"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D112:D116"/>
-    <mergeCell ref="B112:B116"/>
-    <mergeCell ref="D106:D110"/>
+    <mergeCell ref="D76:D81"/>
+    <mergeCell ref="D82:D87"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="D96:D101"/>
+    <mergeCell ref="D108:D113"/>
+    <mergeCell ref="D102:D107"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="B76:B81"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="B96:B101"/>
+    <mergeCell ref="B108:B113"/>
+    <mergeCell ref="B102:B107"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="B114:B119"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="D121:D126"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="D114:D119"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>